<commit_message>
changed the random integer generator to use random instead of a new numpy feature
</commit_message>
<xml_diff>
--- a/summarydataLosAngelesUndetectedCase.xlsx
+++ b/summarydataLosAngelesUndetectedCase.xlsx
@@ -560,10 +560,10 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -580,10 +580,10 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E10">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -600,10 +600,10 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E11">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F11">
         <v>1</v>
@@ -620,10 +620,10 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E12">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -660,13 +660,13 @@
         <v>1</v>
       </c>
       <c r="D14">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E14">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -680,13 +680,13 @@
         <v>1</v>
       </c>
       <c r="D15">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E15">
+        <v>7</v>
+      </c>
+      <c r="F15">
         <v>6</v>
-      </c>
-      <c r="F15">
-        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -700,13 +700,13 @@
         <v>1</v>
       </c>
       <c r="D16">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E16">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F16">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -720,13 +720,13 @@
         <v>1</v>
       </c>
       <c r="D17">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="E17">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="F17">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -740,10 +740,10 @@
         <v>1</v>
       </c>
       <c r="D18">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="E18">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="F18">
         <v>7</v>
@@ -757,16 +757,16 @@
         <v>0</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D19">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="E19">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="F19">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -777,16 +777,16 @@
         <v>0</v>
       </c>
       <c r="C20">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D20">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="E20">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F20">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -797,13 +797,13 @@
         <v>0</v>
       </c>
       <c r="C21">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D21">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="E21">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="F21">
         <v>8</v>
@@ -817,16 +817,16 @@
         <v>0</v>
       </c>
       <c r="C22">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D22">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="E22">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F22">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -834,19 +834,19 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23">
         <v>8</v>
       </c>
       <c r="D23">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="E23">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="F23">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -854,19 +854,19 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C24">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D24">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="E24">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="F24">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -874,19 +874,19 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C25">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D25">
-        <v>60</v>
+        <v>98</v>
       </c>
       <c r="E25">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="F25">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -894,19 +894,19 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C26">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D26">
-        <v>82</v>
+        <v>118</v>
       </c>
       <c r="E26">
-        <v>45</v>
+        <v>73</v>
       </c>
       <c r="F26">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -914,19 +914,19 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C27">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="D27">
-        <v>93</v>
+        <v>141</v>
       </c>
       <c r="E27">
-        <v>52</v>
+        <v>86</v>
       </c>
       <c r="F27">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -934,19 +934,19 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C28">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="D28">
-        <v>116</v>
+        <v>165</v>
       </c>
       <c r="E28">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="F28">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -954,19 +954,19 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C29">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="D29">
-        <v>132</v>
+        <v>191</v>
       </c>
       <c r="E29">
-        <v>81</v>
+        <v>115</v>
       </c>
       <c r="F29">
-        <v>24</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -974,19 +974,19 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C30">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D30">
-        <v>150</v>
+        <v>228</v>
       </c>
       <c r="E30">
-        <v>92</v>
+        <v>137</v>
       </c>
       <c r="F30">
-        <v>25</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -994,19 +994,19 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C31">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="D31">
-        <v>174</v>
+        <v>272</v>
       </c>
       <c r="E31">
-        <v>105</v>
+        <v>165</v>
       </c>
       <c r="F31">
-        <v>32</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1014,19 +1014,19 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C32">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="D32">
-        <v>204</v>
+        <v>326</v>
       </c>
       <c r="E32">
-        <v>117</v>
+        <v>200</v>
       </c>
       <c r="F32">
-        <v>46</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>